<commit_message>
NICK MF Reporting updates
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_3.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_3.xlsx
@@ -18,7 +18,7 @@
     <definedName name="GR_CODE_ROW">4583</definedName>
     <definedName name="GR_CODE_SHEET">4</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ОПСД_3!$A$1:$D$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ОПСД_3!$A$1:$D$43</definedName>
   </definedNames>
   <calcPr calcId="152511" iterateCount="10000" iterateDelta="1E-10"/>
   <extLst>
@@ -290,53 +290,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -657,10 +657,10 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,20 +1312,20 @@
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -1339,318 +1339,304 @@
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="17" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
+      <c r="A14" s="17">
         <v>1</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="17">
         <v>2</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="17">
         <v>3</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="17">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15" s="19">
         <v>1</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A16" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B16" s="19">
         <v>2</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+    </row>
+    <row r="17" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="23">
+        <v>3</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="24">
-        <v>3</v>
-      </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="10"/>
+      <c r="A18" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="21">
+        <v>4</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
     </row>
     <row r="19" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="22">
-        <v>4</v>
-      </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-    </row>
-    <row r="20" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="A19" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B19" s="21">
         <v>5</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="21">
+        <v>6</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="22">
-        <v>6</v>
+    </row>
+    <row r="21" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="23">
+        <v>7</v>
       </c>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
     </row>
-    <row r="22" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="24">
-        <v>7</v>
-      </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-    </row>
-    <row r="24" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+    </row>
+    <row r="23" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="24">
+      <c r="B23" s="23">
         <v>8</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="22">
+      <c r="B24" s="21">
         <v>9</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="21">
+        <v>10</v>
+      </c>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="11"/>
+      <c r="G25" s="9"/>
       <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="22">
-        <v>10</v>
-      </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="11"/>
-      <c r="G26" s="9"/>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
+      <c r="A26" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="24">
+      <c r="B26" s="23">
         <v>11</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-    </row>
-    <row r="28" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+    </row>
+    <row r="27" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="20">
+      <c r="B27" s="19">
         <v>12</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="10"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="10"/>
+      <c r="G27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="19">
+        <v>13</v>
+      </c>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
       <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="10"/>
-      <c r="G29" s="9"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="20">
-        <v>13</v>
-      </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="G30" s="9"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+    </row>
+    <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
+      <c r="A31" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="30" t="s">
-        <v>31</v>
-      </c>
+      <c r="A32" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="29"/>
       <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-    </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
-        <v>32</v>
-      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="29"/>
       <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-    </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="30"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" s="32"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
+      <c r="A37" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="30"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
-      <c r="B38" s="32" t="s">
+      <c r="A38" s="29"/>
+      <c r="B38" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="32"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
+      <c r="A39" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-      <c r="B40" s="32" t="s">
+      <c r="A40" s="29"/>
+      <c r="B40" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
+      <c r="A41" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="30"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
-      <c r="B42" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
+      <c r="A42" s="1"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B43" s="32"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="12"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="12"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C47" s="15"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C48" s="11"/>
+      <c r="C45" s="15"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C46" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A30:D30"/>
     <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
NICK MF Reporting: - report 7 changes
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_3.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_3.xlsx
@@ -15,10 +15,10 @@
     <sheet name="ОПСД_3" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Database">#REF!</definedName>
     <definedName name="GR_CODE_ROW">4583</definedName>
     <definedName name="GR_CODE_SHEET">4</definedName>
-    <definedName name="_xlnm.Database">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ОПСД_3!$A$1:$D$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ОПСД_3!$A$1:$D$42</definedName>
   </definedNames>
   <calcPr calcId="152511" iterateCount="10000" iterateDelta="1E-10"/>
   <extLst>
@@ -149,10 +149,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -252,7 +252,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -273,9 +273,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -286,7 +286,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -340,8 +340,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -657,10 +657,10 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,204 +1439,198 @@
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-    </row>
-    <row r="23" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+    <row r="22" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="23">
+      <c r="B22" s="23">
         <v>8</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="21">
+        <v>9</v>
+      </c>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B24" s="21">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
+      <c r="E24" s="11"/>
+      <c r="G24" s="9"/>
       <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="21">
-        <v>10</v>
-      </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="11"/>
-      <c r="G25" s="9"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A25" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="23">
+      <c r="B25" s="23">
         <v>11</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-    </row>
-    <row r="27" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+    </row>
+    <row r="26" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="19">
+        <v>12</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="10"/>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B27" s="19">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
-      <c r="E27" s="10"/>
       <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="19">
-        <v>13</v>
-      </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-    </row>
-    <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="27"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+    </row>
+    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
       <c r="D31" s="32"/>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-    </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="29"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="29"/>
       <c r="B33" s="30"/>
       <c r="C33" s="29"/>
       <c r="D33" s="29"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
+      <c r="A34" s="29" t="s">
+        <v>33</v>
+      </c>
       <c r="B34" s="30"/>
       <c r="C34" s="29"/>
       <c r="D34" s="29"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="30"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="30" t="s">
+        <v>34</v>
+      </c>
       <c r="C35" s="29"/>
       <c r="D35" s="29"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
-      <c r="B36" s="30" t="s">
-        <v>34</v>
-      </c>
+      <c r="A36" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="30"/>
       <c r="C36" s="29"/>
       <c r="D36" s="29"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="30"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="30" t="s">
+        <v>34</v>
+      </c>
       <c r="C37" s="29"/>
       <c r="D37" s="29"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="29"/>
+      <c r="A38" s="29" t="s">
+        <v>36</v>
+      </c>
       <c r="B38" s="30" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C38" s="29"/>
       <c r="D38" s="29"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="29" t="s">
-        <v>36</v>
-      </c>
+      <c r="A39" s="29"/>
       <c r="B39" s="30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C39" s="29"/>
       <c r="D39" s="29"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
-      <c r="B40" s="30" t="s">
-        <v>34</v>
-      </c>
+      <c r="A40" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="30"/>
       <c r="C40" s="29"/>
       <c r="D40" s="29"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" s="30"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
+      <c r="A41" s="1"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="14"/>
       <c r="D42" s="12"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="12"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="15"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C45" s="15"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C46" s="11"/>
+      <c r="C45" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>